<commit_message>
Commit from GitHub Actions (MainWorkflow)
</commit_message>
<xml_diff>
--- a/reports/metrics.xlsx
+++ b/reports/metrics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,6 +531,62 @@
         <v>0.281001881001881</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>KNN_version_1</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.3217391304347826</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.07035330694830499</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.07430097822851121</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.07126649005254523</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.2836746693384991</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.3217391304347826</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.2985569894858061</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>KNN_version_2</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.2363636363636364</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1128668149459225</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1150636802810716</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.113201041836724</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.2304672457816474</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.2363636363636364</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.2323304717634825</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>